<commit_message>
categori list and janus milestone chain
</commit_message>
<xml_diff>
--- a/xls/template/MDR_Template.xlsx
+++ b/xls/template/MDR_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10909"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11109"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dp/py3/technip/longson/xls/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59233B3A-3E0B-4641-B076-CE49C23F5F18}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28342CE5-7EA6-824A-80E1-F0227F06B066}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="17480" tabRatio="848" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="848" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CPY_Format" sheetId="29" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>REV.</t>
   </si>
@@ -169,6 +169,9 @@
   </si>
   <si>
     <t>CAN = Issue for Cancellation</t>
+  </si>
+  <si>
+    <t>Master Document Index (MDI)</t>
   </si>
 </sst>
 </file>
@@ -554,7 +557,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -581,29 +584,167 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="3" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="17" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="4" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -611,290 +752,144 @@
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="3" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="4" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="17" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="22" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="23" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="11">
@@ -1341,7 +1336,7 @@
       <pane xSplit="7" ySplit="10" topLeftCell="H11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="AI1" sqref="AI1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="F13" sqref="F13"/>
+      <selection pane="bottomRight" activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.5" defaultRowHeight="13"/>
@@ -1349,23 +1344,11 @@
     <col min="1" max="1" width="4.6640625" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4.6640625" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.33203125" style="5" customWidth="1"/>
-    <col min="5" max="5" width="9.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="16.83203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="16.6640625" style="5" customWidth="1"/>
-    <col min="8" max="8" width="14.83203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="13.6640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="17.33203125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="10.1640625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="9.33203125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="10.83203125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="10.6640625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="9.33203125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="9.83203125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="10.5" style="1" customWidth="1"/>
-    <col min="18" max="18" width="12.83203125" style="1" customWidth="1"/>
-    <col min="19" max="19" width="10.5" style="1" customWidth="1"/>
-    <col min="20" max="20" width="10.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="22.5" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="20.1640625" style="5" customWidth="1"/>
+    <col min="8" max="20" width="20.1640625" style="1" customWidth="1"/>
     <col min="21" max="185" width="2.5" style="1"/>
     <col min="186" max="192" width="2.5" style="1" customWidth="1"/>
     <col min="193" max="193" width="2.83203125" style="1" customWidth="1"/>
@@ -2189,342 +2172,326 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="12.75" customHeight="1">
-      <c r="A1" s="45"/>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="75"/>
-      <c r="G1" s="21" t="s">
+      <c r="A1" s="35"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="67" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="68"/>
+      <c r="G1" s="73" t="s">
         <v>33</v>
       </c>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
-      <c r="M1" s="22"/>
-      <c r="N1" s="22"/>
-      <c r="O1" s="22"/>
-      <c r="P1" s="22"/>
-      <c r="Q1" s="74"/>
-      <c r="R1" s="16" t="s">
+      <c r="H1" s="74"/>
+      <c r="I1" s="74"/>
+      <c r="J1" s="74"/>
+      <c r="K1" s="74"/>
+      <c r="L1" s="74"/>
+      <c r="M1" s="74"/>
+      <c r="N1" s="74"/>
+      <c r="O1" s="74"/>
+      <c r="P1" s="74"/>
+      <c r="Q1" s="75"/>
+      <c r="R1" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="S1" s="81"/>
-      <c r="T1" s="58" t="s">
+      <c r="S1" s="56"/>
+      <c r="T1" s="51" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:20" ht="12.75" customHeight="1">
-      <c r="A2" s="47"/>
-      <c r="B2" s="48"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="76"/>
-      <c r="G2" s="23" t="s">
+      <c r="A2" s="37"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="76" t="s">
         <v>30</v>
       </c>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="73"/>
-      <c r="K2" s="23" t="s">
+      <c r="H2" s="77"/>
+      <c r="I2" s="77"/>
+      <c r="J2" s="78"/>
+      <c r="K2" s="76" t="s">
         <v>31</v>
       </c>
-      <c r="L2" s="24"/>
-      <c r="M2" s="24"/>
-      <c r="N2" s="24"/>
-      <c r="O2" s="73"/>
-      <c r="P2" s="23" t="s">
+      <c r="L2" s="77"/>
+      <c r="M2" s="77"/>
+      <c r="N2" s="77"/>
+      <c r="O2" s="78"/>
+      <c r="P2" s="76" t="s">
         <v>32</v>
       </c>
-      <c r="Q2" s="73"/>
-      <c r="R2" s="17"/>
-      <c r="S2" s="82"/>
-      <c r="T2" s="59"/>
+      <c r="Q2" s="78"/>
+      <c r="R2" s="57"/>
+      <c r="S2" s="58"/>
+      <c r="T2" s="52"/>
     </row>
     <row r="3" spans="1:20" ht="12.75" customHeight="1">
-      <c r="A3" s="47"/>
-      <c r="B3" s="48"/>
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="76"/>
-      <c r="G3" s="25" t="s">
+      <c r="A3" s="37"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="69"/>
+      <c r="F3" s="70"/>
+      <c r="G3" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="H3" s="26"/>
-      <c r="I3" s="30" t="s">
+      <c r="H3" s="45"/>
+      <c r="I3" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="J3" s="83"/>
-      <c r="K3" s="54" t="s">
+      <c r="J3" s="22"/>
+      <c r="K3" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="L3" s="30"/>
-      <c r="M3" s="30"/>
-      <c r="N3" s="57" t="s">
+      <c r="L3" s="43"/>
+      <c r="M3" s="43"/>
+      <c r="N3" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="O3" s="92"/>
-      <c r="P3" s="54" t="s">
+      <c r="O3" s="13"/>
+      <c r="P3" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="Q3" s="83"/>
-      <c r="R3" s="12" t="s">
+      <c r="Q3" s="22"/>
+      <c r="R3" s="59" t="s">
         <v>18</v>
       </c>
-      <c r="S3" s="78"/>
-      <c r="T3" s="60" t="s">
+      <c r="S3" s="60"/>
+      <c r="T3" s="47" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:20" ht="12.75" customHeight="1">
-      <c r="A4" s="47"/>
-      <c r="B4" s="48"/>
-      <c r="C4" s="48"/>
-      <c r="D4" s="48"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="76"/>
-      <c r="G4" s="42" t="s">
+      <c r="A4" s="37"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="69"/>
+      <c r="F4" s="70"/>
+      <c r="G4" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="43"/>
-      <c r="I4" s="29" t="s">
+      <c r="H4" s="32"/>
+      <c r="I4" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="J4" s="84"/>
-      <c r="K4" s="53" t="s">
+      <c r="J4" s="19"/>
+      <c r="K4" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="L4" s="31"/>
-      <c r="M4" s="31"/>
-      <c r="N4" s="31" t="s">
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="O4" s="91"/>
-      <c r="P4" s="53" t="s">
+      <c r="O4" s="20"/>
+      <c r="P4" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="Q4" s="91"/>
-      <c r="R4" s="13"/>
-      <c r="S4" s="79"/>
-      <c r="T4" s="61"/>
+      <c r="Q4" s="20"/>
+      <c r="R4" s="61"/>
+      <c r="S4" s="62"/>
+      <c r="T4" s="48"/>
     </row>
     <row r="5" spans="1:20" ht="12.75" customHeight="1">
-      <c r="A5" s="49"/>
-      <c r="B5" s="50"/>
-      <c r="C5" s="50"/>
-      <c r="D5" s="50"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="77"/>
-      <c r="G5" s="42" t="s">
+      <c r="A5" s="39"/>
+      <c r="B5" s="40"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="71"/>
+      <c r="F5" s="72"/>
+      <c r="G5" s="81" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="43"/>
-      <c r="I5" s="28" t="s">
+      <c r="H5" s="82"/>
+      <c r="I5" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="J5" s="85"/>
-      <c r="K5" s="53" t="s">
+      <c r="J5" s="19"/>
+      <c r="K5" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="L5" s="31"/>
-      <c r="M5" s="31"/>
-      <c r="N5" s="31"/>
-      <c r="O5" s="91"/>
-      <c r="P5" s="52" t="s">
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="20"/>
+      <c r="P5" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="Q5" s="84"/>
-      <c r="R5" s="14"/>
-      <c r="S5" s="80"/>
-      <c r="T5" s="62"/>
+      <c r="Q5" s="19"/>
+      <c r="R5" s="63"/>
+      <c r="S5" s="64"/>
+      <c r="T5" s="49"/>
     </row>
     <row r="6" spans="1:20" ht="12.75" customHeight="1">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="50"/>
       <c r="E6" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F6" s="2"/>
-      <c r="G6" s="42" t="s">
+      <c r="G6" s="81" t="s">
         <v>24</v>
       </c>
-      <c r="H6" s="43"/>
-      <c r="I6" s="28" t="s">
+      <c r="H6" s="82"/>
+      <c r="I6" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="J6" s="85"/>
-      <c r="K6" s="51" t="s">
+      <c r="J6" s="19"/>
+      <c r="K6" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="L6" s="32"/>
-      <c r="M6" s="32"/>
-      <c r="N6" s="32"/>
-      <c r="O6" s="90"/>
-      <c r="P6" s="51"/>
-      <c r="Q6" s="90"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="17"/>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="17"/>
       <c r="R6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="S6" s="55"/>
-      <c r="T6" s="63"/>
+      <c r="S6" s="23"/>
+      <c r="T6" s="24"/>
     </row>
     <row r="7" spans="1:20" ht="12.75" customHeight="1">
-      <c r="A7" s="34"/>
-      <c r="B7" s="34"/>
-      <c r="C7" s="34"/>
-      <c r="D7" s="64"/>
-      <c r="E7" s="44"/>
-      <c r="F7" s="87"/>
-      <c r="G7" s="40" t="s">
+      <c r="A7" s="15"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="34"/>
+      <c r="G7" s="81" t="s">
         <v>36</v>
       </c>
-      <c r="H7" s="41"/>
-      <c r="I7" s="28" t="s">
+      <c r="H7" s="82"/>
+      <c r="I7" s="46" t="s">
         <v>39</v>
       </c>
-      <c r="J7" s="85"/>
-      <c r="K7" s="33"/>
-      <c r="L7" s="34"/>
-      <c r="M7" s="34"/>
-      <c r="N7" s="34"/>
-      <c r="O7" s="34"/>
-      <c r="P7" s="34"/>
-      <c r="Q7" s="64"/>
-      <c r="R7" s="55"/>
-      <c r="S7" s="56"/>
-      <c r="T7" s="63"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="15"/>
+      <c r="N7" s="15"/>
+      <c r="O7" s="15"/>
+      <c r="P7" s="15"/>
+      <c r="Q7" s="16"/>
+      <c r="R7" s="23"/>
+      <c r="S7" s="25"/>
+      <c r="T7" s="24"/>
     </row>
     <row r="8" spans="1:20" ht="12.75" customHeight="1">
-      <c r="A8" s="35" t="s">
+      <c r="A8" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="36"/>
-      <c r="C8" s="36"/>
-      <c r="D8" s="89"/>
-      <c r="E8" s="37"/>
-      <c r="F8" s="88"/>
-      <c r="G8" s="38" t="s">
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="83" t="s">
         <v>35</v>
       </c>
-      <c r="H8" s="39"/>
-      <c r="I8" s="27" t="s">
+      <c r="H8" s="84"/>
+      <c r="I8" s="85" t="s">
         <v>40</v>
       </c>
       <c r="J8" s="86"/>
-      <c r="K8" s="8" t="s">
+      <c r="K8" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="L8" s="9"/>
-      <c r="M8" s="9"/>
-      <c r="N8" s="9"/>
-      <c r="O8" s="9"/>
+      <c r="L8" s="42"/>
+      <c r="M8" s="42"/>
+      <c r="N8" s="42"/>
+      <c r="O8" s="42"/>
       <c r="P8" s="6" t="s">
         <v>17</v>
       </c>
       <c r="Q8" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="R8" s="33"/>
-      <c r="S8" s="34"/>
-      <c r="T8" s="64"/>
+      <c r="R8" s="14"/>
+      <c r="S8" s="15"/>
+      <c r="T8" s="16"/>
     </row>
     <row r="9" spans="1:20" ht="12.75" customHeight="1">
-      <c r="A9" s="71" t="s">
+      <c r="A9" s="79" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="69" t="s">
+      <c r="B9" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="69" t="s">
+      <c r="C9" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="87" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="67"/>
-      <c r="F9" s="69" t="s">
+      <c r="E9" s="88"/>
+      <c r="F9" s="65" t="s">
         <v>21</v>
       </c>
-      <c r="G9" s="65"/>
-      <c r="H9" s="65"/>
-      <c r="I9" s="65"/>
-      <c r="J9" s="65"/>
-      <c r="K9" s="65"/>
-      <c r="L9" s="65"/>
-      <c r="M9" s="65"/>
-      <c r="N9" s="65"/>
-      <c r="O9" s="65"/>
-      <c r="P9" s="65"/>
-      <c r="Q9" s="65"/>
-      <c r="R9" s="65"/>
-      <c r="S9" s="65"/>
-      <c r="T9" s="65"/>
+      <c r="G9" s="53"/>
+      <c r="H9" s="53"/>
+      <c r="I9" s="53"/>
+      <c r="J9" s="53"/>
+      <c r="K9" s="53"/>
+      <c r="L9" s="53"/>
+      <c r="M9" s="53"/>
+      <c r="N9" s="53"/>
+      <c r="O9" s="53"/>
+      <c r="P9" s="53"/>
+      <c r="Q9" s="53"/>
+      <c r="R9" s="53"/>
+      <c r="S9" s="53"/>
+      <c r="T9" s="53"/>
     </row>
     <row r="10" spans="1:20" ht="12" customHeight="1">
-      <c r="A10" s="72"/>
-      <c r="B10" s="70"/>
-      <c r="C10" s="70"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="68"/>
-      <c r="F10" s="70"/>
-      <c r="G10" s="66"/>
-      <c r="H10" s="66"/>
-      <c r="I10" s="66"/>
-      <c r="J10" s="66"/>
-      <c r="K10" s="66"/>
-      <c r="L10" s="66"/>
-      <c r="M10" s="66"/>
-      <c r="N10" s="66"/>
-      <c r="O10" s="66"/>
-      <c r="P10" s="66"/>
-      <c r="Q10" s="66"/>
-      <c r="R10" s="66"/>
-      <c r="S10" s="66"/>
-      <c r="T10" s="66"/>
+      <c r="A10" s="80"/>
+      <c r="B10" s="66"/>
+      <c r="C10" s="66"/>
+      <c r="D10" s="89"/>
+      <c r="E10" s="90"/>
+      <c r="F10" s="66"/>
+      <c r="G10" s="54"/>
+      <c r="H10" s="54"/>
+      <c r="I10" s="54"/>
+      <c r="J10" s="54"/>
+      <c r="K10" s="54"/>
+      <c r="L10" s="54"/>
+      <c r="M10" s="54"/>
+      <c r="N10" s="54"/>
+      <c r="O10" s="54"/>
+      <c r="P10" s="54"/>
+      <c r="Q10" s="54"/>
+      <c r="R10" s="54"/>
+      <c r="S10" s="54"/>
+      <c r="T10" s="54"/>
     </row>
   </sheetData>
   <mergeCells count="64">
-    <mergeCell ref="K4:M4"/>
-    <mergeCell ref="K5:M5"/>
-    <mergeCell ref="K6:M6"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="R8:T8"/>
-    <mergeCell ref="P6:Q6"/>
-    <mergeCell ref="P5:Q5"/>
-    <mergeCell ref="P4:Q4"/>
-    <mergeCell ref="P3:Q3"/>
-    <mergeCell ref="S6:T6"/>
-    <mergeCell ref="R7:T7"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="N5:O5"/>
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="K7:Q7"/>
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A1:D5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="K3:M3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="O9:O10"/>
+    <mergeCell ref="P9:P10"/>
+    <mergeCell ref="K8:O8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:E10"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="K9:K10"/>
+    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="N9:N10"/>
     <mergeCell ref="I3:J3"/>
     <mergeCell ref="T3:T5"/>
     <mergeCell ref="C6:D6"/>
@@ -2541,21 +2508,39 @@
     <mergeCell ref="G2:J2"/>
     <mergeCell ref="K2:O2"/>
     <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="O9:O10"/>
-    <mergeCell ref="P9:P10"/>
-    <mergeCell ref="K8:O8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:E10"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="K9:K10"/>
-    <mergeCell ref="L9:L10"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="N9:N10"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A1:D5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="K5:M5"/>
+    <mergeCell ref="K6:M6"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="R8:T8"/>
+    <mergeCell ref="P6:Q6"/>
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="S6:T6"/>
+    <mergeCell ref="R7:T7"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="K7:Q7"/>
+    <mergeCell ref="K3:M3"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>

<commit_message>
full mdi last rev
</commit_message>
<xml_diff>
--- a/xls/template/MDR_Template.xlsx
+++ b/xls/template/MDR_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dp/py3/technip/longson/xls/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28342CE5-7EA6-824A-80E1-F0227F06B066}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6EE607F-DEE0-AA45-B12A-B75BD08D20DD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="848" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="17480" tabRatio="848" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CPY_Format" sheetId="29" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>REV.</t>
   </si>
@@ -46,9 +46,6 @@
     <t>Owner:</t>
   </si>
   <si>
-    <t>Plant Name:</t>
-  </si>
-  <si>
     <t>Issue Date</t>
   </si>
   <si>
@@ -172,6 +169,15 @@
   </si>
   <si>
     <t>Master Document Index (MDI)</t>
+  </si>
+  <si>
+    <t>Long Son Pterochemicals C0., Ltd.</t>
+  </si>
+  <si>
+    <t>Plant Name: PACKAGE A1: OLEFINS PLANT</t>
+  </si>
+  <si>
+    <t>Att. To OL1-2W91-0001 036909C-1000-NM-107</t>
   </si>
 </sst>
 </file>
@@ -557,15 +563,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
@@ -584,31 +586,190 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -617,76 +778,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="3" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="17" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="4" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -714,156 +805,31 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -871,25 +837,69 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="3" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="17" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="4" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="11">
@@ -1336,18 +1346,18 @@
       <pane xSplit="7" ySplit="10" topLeftCell="H11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="AI1" sqref="AI1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="F14" sqref="F14"/>
+      <selection pane="bottomRight" activeCell="F9" sqref="F9:F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.5" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="4.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.6640625" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.6640625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" style="4" customWidth="1"/>
     <col min="5" max="5" width="22.5" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="20.1640625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="15.83203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="20.1640625" style="4" customWidth="1"/>
     <col min="8" max="20" width="20.1640625" style="1" customWidth="1"/>
     <col min="21" max="185" width="2.5" style="1"/>
     <col min="186" max="192" width="2.5" style="1" customWidth="1"/>
@@ -2172,326 +2182,348 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="12.75" customHeight="1">
-      <c r="A1" s="35"/>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="67" t="s">
-        <v>41</v>
-      </c>
-      <c r="F1" s="68"/>
-      <c r="G1" s="73" t="s">
-        <v>33</v>
-      </c>
-      <c r="H1" s="74"/>
-      <c r="I1" s="74"/>
-      <c r="J1" s="74"/>
-      <c r="K1" s="74"/>
-      <c r="L1" s="74"/>
-      <c r="M1" s="74"/>
-      <c r="N1" s="74"/>
-      <c r="O1" s="74"/>
-      <c r="P1" s="74"/>
-      <c r="Q1" s="75"/>
-      <c r="R1" s="55" t="s">
+      <c r="A1" s="61"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="37" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" s="38"/>
+      <c r="G1" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
+      <c r="M1" s="44"/>
+      <c r="N1" s="44"/>
+      <c r="O1" s="44"/>
+      <c r="P1" s="44"/>
+      <c r="Q1" s="45"/>
+      <c r="R1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="S1" s="56"/>
-      <c r="T1" s="51" t="s">
+      <c r="S1" s="28"/>
+      <c r="T1" s="25" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:20" ht="12.75" customHeight="1">
-      <c r="A2" s="37"/>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="69"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="76" t="s">
+      <c r="A2" s="63"/>
+      <c r="B2" s="64"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="46" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="47"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="48"/>
+      <c r="K2" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="H2" s="77"/>
-      <c r="I2" s="77"/>
-      <c r="J2" s="78"/>
-      <c r="K2" s="76" t="s">
+      <c r="L2" s="47"/>
+      <c r="M2" s="47"/>
+      <c r="N2" s="47"/>
+      <c r="O2" s="48"/>
+      <c r="P2" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="L2" s="77"/>
-      <c r="M2" s="77"/>
-      <c r="N2" s="77"/>
-      <c r="O2" s="78"/>
-      <c r="P2" s="76" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q2" s="78"/>
-      <c r="R2" s="57"/>
-      <c r="S2" s="58"/>
-      <c r="T2" s="52"/>
+      <c r="Q2" s="48"/>
+      <c r="R2" s="29"/>
+      <c r="S2" s="30"/>
+      <c r="T2" s="26"/>
     </row>
     <row r="3" spans="1:20" ht="12.75" customHeight="1">
-      <c r="A3" s="37"/>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="69"/>
-      <c r="F3" s="70"/>
-      <c r="G3" s="44" t="s">
-        <v>34</v>
-      </c>
-      <c r="H3" s="45"/>
-      <c r="I3" s="43" t="s">
-        <v>25</v>
-      </c>
-      <c r="J3" s="22"/>
-      <c r="K3" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="L3" s="43"/>
-      <c r="M3" s="43"/>
-      <c r="N3" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="O3" s="13"/>
-      <c r="P3" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q3" s="22"/>
-      <c r="R3" s="59" t="s">
+      <c r="A3" s="63"/>
+      <c r="B3" s="64"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="67" t="s">
+        <v>33</v>
+      </c>
+      <c r="H3" s="68"/>
+      <c r="I3" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" s="20"/>
+      <c r="K3" s="86" t="s">
+        <v>21</v>
+      </c>
+      <c r="L3" s="19"/>
+      <c r="M3" s="19"/>
+      <c r="N3" s="80" t="s">
+        <v>14</v>
+      </c>
+      <c r="O3" s="81"/>
+      <c r="P3" s="86" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q3" s="20"/>
+      <c r="R3" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="S3" s="32"/>
+      <c r="T3" s="21" t="s">
         <v>18</v>
-      </c>
-      <c r="S3" s="60"/>
-      <c r="T3" s="47" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:20" ht="12.75" customHeight="1">
-      <c r="A4" s="37"/>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="69"/>
-      <c r="F4" s="70"/>
-      <c r="G4" s="31" t="s">
-        <v>23</v>
-      </c>
-      <c r="H4" s="32"/>
-      <c r="I4" s="46" t="s">
-        <v>26</v>
-      </c>
-      <c r="J4" s="19"/>
-      <c r="K4" s="8" t="s">
+      <c r="A4" s="63"/>
+      <c r="B4" s="64"/>
+      <c r="C4" s="64"/>
+      <c r="D4" s="64"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="55" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="56"/>
+      <c r="I4" s="51" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" s="52"/>
+      <c r="K4" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="L4" s="9"/>
-      <c r="M4" s="9"/>
-      <c r="N4" s="9" t="s">
+      <c r="L4" s="77"/>
+      <c r="M4" s="77"/>
+      <c r="N4" s="77" t="s">
         <v>3</v>
       </c>
-      <c r="O4" s="20"/>
-      <c r="P4" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q4" s="20"/>
-      <c r="R4" s="61"/>
-      <c r="S4" s="62"/>
-      <c r="T4" s="48"/>
+      <c r="O4" s="85"/>
+      <c r="P4" s="76" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q4" s="85"/>
+      <c r="R4" s="33"/>
+      <c r="S4" s="34"/>
+      <c r="T4" s="22"/>
     </row>
     <row r="5" spans="1:20" ht="12.75" customHeight="1">
-      <c r="A5" s="39"/>
-      <c r="B5" s="40"/>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="71"/>
-      <c r="F5" s="72"/>
-      <c r="G5" s="81" t="s">
-        <v>20</v>
-      </c>
-      <c r="H5" s="82"/>
-      <c r="I5" s="46" t="s">
-        <v>37</v>
-      </c>
-      <c r="J5" s="19"/>
-      <c r="K5" s="8" t="s">
+      <c r="A5" s="65"/>
+      <c r="B5" s="66"/>
+      <c r="C5" s="66"/>
+      <c r="D5" s="66"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="53" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="54"/>
+      <c r="I5" s="51" t="s">
+        <v>36</v>
+      </c>
+      <c r="J5" s="52"/>
+      <c r="K5" s="76" t="s">
         <v>4</v>
       </c>
-      <c r="L5" s="9"/>
-      <c r="M5" s="9"/>
-      <c r="N5" s="9"/>
-      <c r="O5" s="20"/>
-      <c r="P5" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q5" s="19"/>
-      <c r="R5" s="63"/>
-      <c r="S5" s="64"/>
-      <c r="T5" s="49"/>
+      <c r="L5" s="77"/>
+      <c r="M5" s="77"/>
+      <c r="N5" s="77"/>
+      <c r="O5" s="85"/>
+      <c r="P5" s="84" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q5" s="52"/>
+      <c r="R5" s="35"/>
+      <c r="S5" s="36"/>
+      <c r="T5" s="23"/>
     </row>
     <row r="6" spans="1:20" ht="12.75" customHeight="1">
-      <c r="A6" s="41" t="s">
+      <c r="A6" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="42"/>
-      <c r="C6" s="50"/>
-      <c r="D6" s="50"/>
-      <c r="E6" s="2" t="s">
+      <c r="B6" s="10"/>
+      <c r="C6" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" s="24"/>
+      <c r="E6" s="90" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" s="91"/>
+      <c r="G6" s="53" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6" s="54"/>
+      <c r="I6" s="51" t="s">
+        <v>37</v>
+      </c>
+      <c r="J6" s="52"/>
+      <c r="K6" s="78" t="s">
+        <v>15</v>
+      </c>
+      <c r="L6" s="79"/>
+      <c r="M6" s="79"/>
+      <c r="N6" s="79"/>
+      <c r="O6" s="83"/>
+      <c r="P6" s="78"/>
+      <c r="Q6" s="83"/>
+      <c r="R6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="2"/>
-      <c r="G6" s="81" t="s">
-        <v>24</v>
-      </c>
-      <c r="H6" s="82"/>
-      <c r="I6" s="46" t="s">
-        <v>38</v>
-      </c>
-      <c r="J6" s="19"/>
-      <c r="K6" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="L6" s="11"/>
-      <c r="M6" s="11"/>
-      <c r="N6" s="11"/>
-      <c r="O6" s="17"/>
-      <c r="P6" s="10"/>
-      <c r="Q6" s="17"/>
-      <c r="R6" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="S6" s="23"/>
-      <c r="T6" s="24"/>
+      <c r="S6" s="87"/>
+      <c r="T6" s="88"/>
     </row>
     <row r="7" spans="1:20" ht="12.75" customHeight="1">
-      <c r="A7" s="15"/>
-      <c r="B7" s="15"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="34"/>
-      <c r="G7" s="81" t="s">
-        <v>36</v>
-      </c>
-      <c r="H7" s="82"/>
-      <c r="I7" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="J7" s="19"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="15"/>
-      <c r="M7" s="15"/>
-      <c r="N7" s="15"/>
-      <c r="O7" s="15"/>
-      <c r="P7" s="15"/>
-      <c r="Q7" s="16"/>
-      <c r="R7" s="23"/>
-      <c r="S7" s="25"/>
-      <c r="T7" s="24"/>
+      <c r="A7" s="59"/>
+      <c r="B7" s="59"/>
+      <c r="C7" s="59"/>
+      <c r="D7" s="60"/>
+      <c r="E7" s="57" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" s="58"/>
+      <c r="G7" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="H7" s="54"/>
+      <c r="I7" s="51" t="s">
+        <v>38</v>
+      </c>
+      <c r="J7" s="52"/>
+      <c r="K7" s="82"/>
+      <c r="L7" s="59"/>
+      <c r="M7" s="59"/>
+      <c r="N7" s="59"/>
+      <c r="O7" s="59"/>
+      <c r="P7" s="59"/>
+      <c r="Q7" s="60"/>
+      <c r="R7" s="87"/>
+      <c r="S7" s="89"/>
+      <c r="T7" s="88"/>
     </row>
     <row r="8" spans="1:20" ht="12.75" customHeight="1">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="69" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="70"/>
+      <c r="C8" s="70"/>
+      <c r="D8" s="71"/>
+      <c r="E8" s="72"/>
+      <c r="F8" s="73"/>
+      <c r="G8" s="74" t="s">
+        <v>34</v>
+      </c>
+      <c r="H8" s="75"/>
+      <c r="I8" s="49" t="s">
+        <v>39</v>
+      </c>
+      <c r="J8" s="50"/>
+      <c r="K8" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="27"/>
-      <c r="C8" s="27"/>
-      <c r="D8" s="28"/>
-      <c r="E8" s="29"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="83" t="s">
-        <v>35</v>
-      </c>
-      <c r="H8" s="84"/>
-      <c r="I8" s="85" t="s">
-        <v>40</v>
-      </c>
-      <c r="J8" s="86"/>
-      <c r="K8" s="41" t="s">
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="10"/>
+      <c r="O8" s="10"/>
+      <c r="P8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="L8" s="42"/>
-      <c r="M8" s="42"/>
-      <c r="N8" s="42"/>
-      <c r="O8" s="42"/>
-      <c r="P8" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q8" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="R8" s="14"/>
-      <c r="S8" s="15"/>
-      <c r="T8" s="16"/>
+      <c r="R8" s="82"/>
+      <c r="S8" s="59"/>
+      <c r="T8" s="60"/>
     </row>
     <row r="9" spans="1:20" ht="12.75" customHeight="1">
-      <c r="A9" s="79" t="s">
+      <c r="A9" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="65" t="s">
+      <c r="C9" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="65" t="s">
+      <c r="D9" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="87" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="88"/>
-      <c r="F9" s="65" t="s">
-        <v>21</v>
-      </c>
-      <c r="G9" s="53"/>
-      <c r="H9" s="53"/>
-      <c r="I9" s="53"/>
-      <c r="J9" s="53"/>
-      <c r="K9" s="53"/>
-      <c r="L9" s="53"/>
-      <c r="M9" s="53"/>
-      <c r="N9" s="53"/>
-      <c r="O9" s="53"/>
-      <c r="P9" s="53"/>
-      <c r="Q9" s="53"/>
-      <c r="R9" s="53"/>
-      <c r="S9" s="53"/>
-      <c r="T9" s="53"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="7"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="7"/>
+      <c r="R9" s="7"/>
+      <c r="S9" s="7"/>
+      <c r="T9" s="7"/>
     </row>
     <row r="10" spans="1:20" ht="12" customHeight="1">
-      <c r="A10" s="80"/>
-      <c r="B10" s="66"/>
-      <c r="C10" s="66"/>
-      <c r="D10" s="89"/>
-      <c r="E10" s="90"/>
-      <c r="F10" s="66"/>
-      <c r="G10" s="54"/>
-      <c r="H10" s="54"/>
-      <c r="I10" s="54"/>
-      <c r="J10" s="54"/>
-      <c r="K10" s="54"/>
-      <c r="L10" s="54"/>
-      <c r="M10" s="54"/>
-      <c r="N10" s="54"/>
-      <c r="O10" s="54"/>
-      <c r="P10" s="54"/>
-      <c r="Q10" s="54"/>
-      <c r="R10" s="54"/>
-      <c r="S10" s="54"/>
-      <c r="T10" s="54"/>
+      <c r="A10" s="12"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="8"/>
+      <c r="P10" s="8"/>
+      <c r="Q10" s="8"/>
+      <c r="R10" s="8"/>
+      <c r="S10" s="8"/>
+      <c r="T10" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="64">
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="O9:O10"/>
-    <mergeCell ref="P9:P10"/>
-    <mergeCell ref="K8:O8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:E10"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="K9:K10"/>
-    <mergeCell ref="L9:L10"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="N9:N10"/>
+  <mergeCells count="65">
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="K5:M5"/>
+    <mergeCell ref="K6:M6"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="R8:T8"/>
+    <mergeCell ref="P6:Q6"/>
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="S6:T6"/>
+    <mergeCell ref="R7:T7"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="K7:Q7"/>
+    <mergeCell ref="K3:M3"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A1:D5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G4:H4"/>
     <mergeCell ref="I3:J3"/>
     <mergeCell ref="T3:T5"/>
     <mergeCell ref="C6:D6"/>
@@ -2508,39 +2540,22 @@
     <mergeCell ref="G2:J2"/>
     <mergeCell ref="K2:O2"/>
     <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="O9:O10"/>
+    <mergeCell ref="P9:P10"/>
+    <mergeCell ref="K8:O8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:E10"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="K9:K10"/>
+    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="N9:N10"/>
     <mergeCell ref="I8:J8"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A1:D5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="K4:M4"/>
-    <mergeCell ref="K5:M5"/>
-    <mergeCell ref="K6:M6"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="R8:T8"/>
-    <mergeCell ref="P6:Q6"/>
-    <mergeCell ref="P5:Q5"/>
-    <mergeCell ref="P4:Q4"/>
-    <mergeCell ref="P3:Q3"/>
-    <mergeCell ref="S6:T6"/>
-    <mergeCell ref="R7:T7"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="N5:O5"/>
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="K7:Q7"/>
-    <mergeCell ref="K3:M3"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>

<commit_message>
fix 13 revision for doc in mdi
</commit_message>
<xml_diff>
--- a/xls/template/MDR_Template.xlsx
+++ b/xls/template/MDR_Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dp/py3/technip/longson/xls/template/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dp/longson/xls/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1F77678-C63A-B74D-BE86-D3EB3F0D9ADE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{329FD562-6091-054F-9D87-92A4130F7309}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="17480" tabRatio="848" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -82,10 +82,6 @@
     <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
-    <t>LSP-2W91-0001</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
     <t>A</t>
     <phoneticPr fontId="9" type="noConversion"/>
   </si>
@@ -178,6 +174,9 @@
   </si>
   <si>
     <t>Att. To OL1-2W91-0001 036909C-1000-NM-107</t>
+  </si>
+  <si>
+    <t>OL1-2W91-0001</t>
   </si>
 </sst>
 </file>
@@ -586,99 +585,232 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="3" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="17" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="4" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -686,12 +818,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -710,195 +836,68 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="3" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="17" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="4" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1343,10 +1342,10 @@
   <dimension ref="A1:T10"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="210" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <pane xSplit="7" ySplit="10" topLeftCell="H11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="10" topLeftCell="I11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="AI1" sqref="AI1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="D14" sqref="D14"/>
+      <selection pane="bottomRight" activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.5" defaultRowHeight="13"/>
@@ -2182,330 +2181,348 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="12.75" customHeight="1">
-      <c r="A1" s="39"/>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="72" t="s">
-        <v>40</v>
-      </c>
-      <c r="F1" s="73"/>
-      <c r="G1" s="78" t="s">
-        <v>32</v>
-      </c>
-      <c r="H1" s="79"/>
-      <c r="I1" s="79"/>
-      <c r="J1" s="79"/>
-      <c r="K1" s="79"/>
-      <c r="L1" s="79"/>
-      <c r="M1" s="79"/>
-      <c r="N1" s="79"/>
-      <c r="O1" s="79"/>
-      <c r="P1" s="79"/>
-      <c r="Q1" s="80"/>
-      <c r="R1" s="60" t="s">
+      <c r="A1" s="49"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" s="38"/>
+      <c r="G1" s="43" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
+      <c r="M1" s="44"/>
+      <c r="N1" s="44"/>
+      <c r="O1" s="44"/>
+      <c r="P1" s="44"/>
+      <c r="Q1" s="45"/>
+      <c r="R1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="S1" s="61"/>
-      <c r="T1" s="56" t="s">
+      <c r="S1" s="28"/>
+      <c r="T1" s="25" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:20" ht="12.75" customHeight="1">
-      <c r="A2" s="41"/>
-      <c r="B2" s="42"/>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="74"/>
-      <c r="F2" s="75"/>
-      <c r="G2" s="81" t="s">
+      <c r="A2" s="51"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="46" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" s="47"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="48"/>
+      <c r="K2" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="H2" s="82"/>
-      <c r="I2" s="82"/>
-      <c r="J2" s="83"/>
-      <c r="K2" s="81" t="s">
+      <c r="L2" s="47"/>
+      <c r="M2" s="47"/>
+      <c r="N2" s="47"/>
+      <c r="O2" s="48"/>
+      <c r="P2" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="L2" s="82"/>
-      <c r="M2" s="82"/>
-      <c r="N2" s="82"/>
-      <c r="O2" s="83"/>
-      <c r="P2" s="81" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q2" s="83"/>
-      <c r="R2" s="62"/>
-      <c r="S2" s="63"/>
-      <c r="T2" s="57"/>
+      <c r="Q2" s="48"/>
+      <c r="R2" s="29"/>
+      <c r="S2" s="30"/>
+      <c r="T2" s="26"/>
     </row>
     <row r="3" spans="1:20" ht="12.75" customHeight="1">
-      <c r="A3" s="41"/>
-      <c r="B3" s="42"/>
-      <c r="C3" s="42"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="74"/>
-      <c r="F3" s="75"/>
-      <c r="G3" s="47" t="s">
-        <v>33</v>
-      </c>
-      <c r="H3" s="48"/>
-      <c r="I3" s="25" t="s">
-        <v>24</v>
-      </c>
-      <c r="J3" s="21"/>
-      <c r="K3" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="L3" s="25"/>
-      <c r="M3" s="25"/>
-      <c r="N3" s="11" t="s">
+      <c r="A3" s="51"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="55" t="s">
+        <v>32</v>
+      </c>
+      <c r="H3" s="56"/>
+      <c r="I3" s="63" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" s="64"/>
+      <c r="K3" s="88" t="s">
+        <v>20</v>
+      </c>
+      <c r="L3" s="63"/>
+      <c r="M3" s="63"/>
+      <c r="N3" s="82" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="12"/>
-      <c r="P3" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q3" s="21"/>
-      <c r="R3" s="64" t="s">
+      <c r="O3" s="83"/>
+      <c r="P3" s="88" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q3" s="64"/>
+      <c r="R3" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="S3" s="32"/>
+      <c r="T3" s="21" t="s">
         <v>17</v>
-      </c>
-      <c r="S3" s="65"/>
-      <c r="T3" s="52" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:20" ht="12.75" customHeight="1">
-      <c r="A4" s="41"/>
-      <c r="B4" s="42"/>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="74"/>
-      <c r="F4" s="75"/>
-      <c r="G4" s="50" t="s">
-        <v>22</v>
-      </c>
-      <c r="H4" s="51"/>
-      <c r="I4" s="49" t="s">
-        <v>25</v>
-      </c>
-      <c r="J4" s="18"/>
-      <c r="K4" s="7" t="s">
+      <c r="A4" s="51"/>
+      <c r="B4" s="52"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="61" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="62"/>
+      <c r="I4" s="57" t="s">
+        <v>24</v>
+      </c>
+      <c r="J4" s="58"/>
+      <c r="K4" s="78" t="s">
         <v>2</v>
       </c>
-      <c r="L4" s="8"/>
-      <c r="M4" s="8"/>
-      <c r="N4" s="8" t="s">
+      <c r="L4" s="79"/>
+      <c r="M4" s="79"/>
+      <c r="N4" s="79" t="s">
         <v>3</v>
       </c>
-      <c r="O4" s="19"/>
-      <c r="P4" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q4" s="19"/>
-      <c r="R4" s="66"/>
-      <c r="S4" s="67"/>
-      <c r="T4" s="53"/>
+      <c r="O4" s="87"/>
+      <c r="P4" s="78" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q4" s="87"/>
+      <c r="R4" s="33"/>
+      <c r="S4" s="34"/>
+      <c r="T4" s="22"/>
     </row>
     <row r="5" spans="1:20" ht="12.75" customHeight="1">
-      <c r="A5" s="43"/>
-      <c r="B5" s="44"/>
-      <c r="C5" s="44"/>
-      <c r="D5" s="44"/>
-      <c r="E5" s="76"/>
-      <c r="F5" s="77"/>
-      <c r="G5" s="33" t="s">
-        <v>19</v>
-      </c>
-      <c r="H5" s="34"/>
-      <c r="I5" s="49" t="s">
-        <v>36</v>
-      </c>
-      <c r="J5" s="18"/>
-      <c r="K5" s="7" t="s">
+      <c r="A5" s="53"/>
+      <c r="B5" s="54"/>
+      <c r="C5" s="54"/>
+      <c r="D5" s="54"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="59" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="60"/>
+      <c r="I5" s="57" t="s">
+        <v>35</v>
+      </c>
+      <c r="J5" s="58"/>
+      <c r="K5" s="78" t="s">
         <v>4</v>
       </c>
-      <c r="L5" s="8"/>
-      <c r="M5" s="8"/>
-      <c r="N5" s="8"/>
-      <c r="O5" s="19"/>
-      <c r="P5" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q5" s="18"/>
-      <c r="R5" s="68"/>
-      <c r="S5" s="69"/>
-      <c r="T5" s="54"/>
+      <c r="L5" s="79"/>
+      <c r="M5" s="79"/>
+      <c r="N5" s="79"/>
+      <c r="O5" s="87"/>
+      <c r="P5" s="86" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q5" s="58"/>
+      <c r="R5" s="35"/>
+      <c r="S5" s="36"/>
+      <c r="T5" s="23"/>
     </row>
     <row r="6" spans="1:20" ht="12.75" customHeight="1">
-      <c r="A6" s="45" t="s">
+      <c r="A6" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="46"/>
-      <c r="C6" s="55" t="s">
+      <c r="B6" s="10"/>
+      <c r="C6" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="24"/>
+      <c r="E6" s="72" t="s">
         <v>41</v>
       </c>
-      <c r="D6" s="55"/>
-      <c r="E6" s="35" t="s">
-        <v>42</v>
-      </c>
-      <c r="F6" s="36"/>
-      <c r="G6" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="H6" s="34"/>
-      <c r="I6" s="49" t="s">
-        <v>37</v>
-      </c>
-      <c r="J6" s="18"/>
-      <c r="K6" s="9" t="s">
+      <c r="F6" s="73"/>
+      <c r="G6" s="59" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="60"/>
+      <c r="I6" s="57" t="s">
+        <v>36</v>
+      </c>
+      <c r="J6" s="58"/>
+      <c r="K6" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="L6" s="10"/>
-      <c r="M6" s="10"/>
-      <c r="N6" s="10"/>
-      <c r="O6" s="16"/>
-      <c r="P6" s="9"/>
-      <c r="Q6" s="16"/>
+      <c r="L6" s="81"/>
+      <c r="M6" s="81"/>
+      <c r="N6" s="81"/>
+      <c r="O6" s="85"/>
+      <c r="P6" s="80"/>
+      <c r="Q6" s="85"/>
       <c r="R6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="S6" s="22"/>
-      <c r="T6" s="23"/>
+      <c r="S6" s="89"/>
+      <c r="T6" s="90"/>
     </row>
     <row r="7" spans="1:20" ht="12.75" customHeight="1">
-      <c r="A7" s="14"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="37" t="s">
-        <v>43</v>
-      </c>
-      <c r="F7" s="38"/>
-      <c r="G7" s="33" t="s">
-        <v>35</v>
-      </c>
-      <c r="H7" s="34"/>
-      <c r="I7" s="49" t="s">
-        <v>38</v>
-      </c>
-      <c r="J7" s="18"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="14"/>
-      <c r="M7" s="14"/>
-      <c r="N7" s="14"/>
-      <c r="O7" s="14"/>
-      <c r="P7" s="14"/>
-      <c r="Q7" s="15"/>
-      <c r="R7" s="22"/>
-      <c r="S7" s="24"/>
-      <c r="T7" s="23"/>
+      <c r="A7" s="76"/>
+      <c r="B7" s="76"/>
+      <c r="C7" s="76"/>
+      <c r="D7" s="77"/>
+      <c r="E7" s="74" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" s="75"/>
+      <c r="G7" s="59" t="s">
+        <v>34</v>
+      </c>
+      <c r="H7" s="60"/>
+      <c r="I7" s="57" t="s">
+        <v>37</v>
+      </c>
+      <c r="J7" s="58"/>
+      <c r="K7" s="84"/>
+      <c r="L7" s="76"/>
+      <c r="M7" s="76"/>
+      <c r="N7" s="76"/>
+      <c r="O7" s="76"/>
+      <c r="P7" s="76"/>
+      <c r="Q7" s="77"/>
+      <c r="R7" s="89"/>
+      <c r="S7" s="91"/>
+      <c r="T7" s="90"/>
     </row>
     <row r="8" spans="1:20" ht="12.75" customHeight="1">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="65" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="27"/>
-      <c r="C8" s="27"/>
-      <c r="D8" s="28"/>
-      <c r="E8" s="29"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="H8" s="32"/>
-      <c r="I8" s="90" t="s">
-        <v>39</v>
-      </c>
-      <c r="J8" s="91"/>
-      <c r="K8" s="45" t="s">
+      <c r="B8" s="66"/>
+      <c r="C8" s="66"/>
+      <c r="D8" s="67"/>
+      <c r="E8" s="68"/>
+      <c r="F8" s="69"/>
+      <c r="G8" s="70" t="s">
+        <v>33</v>
+      </c>
+      <c r="H8" s="71"/>
+      <c r="I8" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="J8" s="20"/>
+      <c r="K8" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="L8" s="46"/>
-      <c r="M8" s="46"/>
-      <c r="N8" s="46"/>
-      <c r="O8" s="46"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="10"/>
+      <c r="O8" s="10"/>
       <c r="P8" s="5" t="s">
         <v>16</v>
       </c>
       <c r="Q8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="R8" s="13"/>
-      <c r="S8" s="14"/>
-      <c r="T8" s="15"/>
+      <c r="R8" s="84"/>
+      <c r="S8" s="76"/>
+      <c r="T8" s="77"/>
     </row>
     <row r="9" spans="1:20" ht="12.75" customHeight="1">
-      <c r="A9" s="84" t="s">
+      <c r="A9" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="70" t="s">
+      <c r="B9" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="70" t="s">
+      <c r="C9" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="86" t="s">
+      <c r="D9" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="87"/>
-      <c r="F9" s="70" t="s">
-        <v>20</v>
-      </c>
-      <c r="G9" s="58"/>
-      <c r="H9" s="58"/>
-      <c r="I9" s="58"/>
-      <c r="J9" s="58"/>
-      <c r="K9" s="58"/>
-      <c r="L9" s="58"/>
-      <c r="M9" s="58"/>
-      <c r="N9" s="58"/>
-      <c r="O9" s="58"/>
-      <c r="P9" s="58"/>
-      <c r="Q9" s="58"/>
-      <c r="R9" s="58"/>
-      <c r="S9" s="58"/>
-      <c r="T9" s="58"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="7"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="7"/>
+      <c r="R9" s="7"/>
+      <c r="S9" s="7"/>
+      <c r="T9" s="7"/>
     </row>
     <row r="10" spans="1:20" ht="12" customHeight="1">
-      <c r="A10" s="85"/>
-      <c r="B10" s="71"/>
-      <c r="C10" s="71"/>
-      <c r="D10" s="88"/>
-      <c r="E10" s="89"/>
-      <c r="F10" s="71"/>
-      <c r="G10" s="59"/>
-      <c r="H10" s="59"/>
-      <c r="I10" s="59"/>
-      <c r="J10" s="59"/>
-      <c r="K10" s="59"/>
-      <c r="L10" s="59"/>
-      <c r="M10" s="59"/>
-      <c r="N10" s="59"/>
-      <c r="O10" s="59"/>
-      <c r="P10" s="59"/>
-      <c r="Q10" s="59"/>
-      <c r="R10" s="59"/>
-      <c r="S10" s="59"/>
-      <c r="T10" s="59"/>
+      <c r="A10" s="12"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="8"/>
+      <c r="P10" s="8"/>
+      <c r="Q10" s="8"/>
+      <c r="R10" s="8"/>
+      <c r="S10" s="8"/>
+      <c r="T10" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="65">
-    <mergeCell ref="O9:O10"/>
-    <mergeCell ref="P9:P10"/>
-    <mergeCell ref="K8:O8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:E10"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="K9:K10"/>
-    <mergeCell ref="L9:L10"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="N9:N10"/>
-    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="K5:M5"/>
+    <mergeCell ref="K6:M6"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="R8:T8"/>
+    <mergeCell ref="P6:Q6"/>
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="S6:T6"/>
+    <mergeCell ref="R7:T7"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="K7:Q7"/>
+    <mergeCell ref="K3:M3"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="A1:D5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="A7:D7"/>
     <mergeCell ref="T3:T5"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="T1:T2"/>
@@ -2522,40 +2539,22 @@
     <mergeCell ref="K2:O2"/>
     <mergeCell ref="P2:Q2"/>
     <mergeCell ref="H9:H10"/>
-    <mergeCell ref="A1:D5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="O9:O10"/>
+    <mergeCell ref="P9:P10"/>
+    <mergeCell ref="K8:O8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:E10"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="K9:K10"/>
+    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="N9:N10"/>
+    <mergeCell ref="I8:J8"/>
     <mergeCell ref="A8:D8"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="K4:M4"/>
-    <mergeCell ref="K5:M5"/>
-    <mergeCell ref="K6:M6"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="R8:T8"/>
-    <mergeCell ref="P6:Q6"/>
-    <mergeCell ref="P5:Q5"/>
-    <mergeCell ref="P4:Q4"/>
-    <mergeCell ref="P3:Q3"/>
-    <mergeCell ref="S6:T6"/>
-    <mergeCell ref="R7:T7"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="N5:O5"/>
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="K7:Q7"/>
-    <mergeCell ref="K3:M3"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>